<commit_message>
Add performance info to the final report
</commit_message>
<xml_diff>
--- a/Report/results.xlsx
+++ b/Report/results.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GriGri\Documents\Projects\FibHeap\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -39,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -539,24 +534,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -596,7 +591,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -645,26 +640,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1303,7 +1278,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D233-48C4-8B63-7E12D331A572}"/>
             </c:ext>
@@ -1940,7 +1915,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D233-48C4-8B63-7E12D331A572}"/>
             </c:ext>
@@ -1954,12 +1929,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="416608904"/>
-        <c:axId val="416610544"/>
+        <c:axId val="73457024"/>
+        <c:axId val="79898112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="416608904"/>
+        <c:axId val="73457024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,26 +1977,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2056,10 +2012,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="416610544"/>
+        <c:crossAx val="79898112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2067,7 +2023,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="416610544"/>
+        <c:axId val="79898112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,26 +2083,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2176,10 +2112,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="416608904"/>
+        <c:crossAx val="73457024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2219,7 +2155,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2249,7 +2185,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2261,7 +2197,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2301,7 +2237,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2942,7 +2878,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ED9E-4545-BC54-D9C60EF8B3C2}"/>
             </c:ext>
@@ -2956,17 +2892,37 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="539295520"/>
-        <c:axId val="539286336"/>
+        <c:axId val="79944320"/>
+        <c:axId val="79946112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="539295520"/>
+        <c:axId val="79944320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3001,10 +2957,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539286336"/>
+        <c:crossAx val="79946112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3012,7 +2968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539286336"/>
+        <c:axId val="79946112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3032,6 +2988,25 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Ticks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3060,10 +3035,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539295520"/>
+        <c:crossAx val="79944320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3103,7 +3078,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3133,7 +3108,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3145,7 +3120,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3185,7 +3160,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3826,7 +3801,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ED9E-4545-BC54-D9C60EF8B3C2}"/>
             </c:ext>
@@ -3840,17 +3815,37 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="539295520"/>
-        <c:axId val="539286336"/>
+        <c:axId val="80110336"/>
+        <c:axId val="80111872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="539295520"/>
+        <c:axId val="80110336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3885,10 +3880,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539286336"/>
+        <c:crossAx val="80111872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3896,7 +3891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539286336"/>
+        <c:axId val="80111872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3916,6 +3911,32 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Ticks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.27253864100320796"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3944,10 +3965,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539295520"/>
+        <c:crossAx val="80110336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3987,7 +4008,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4017,7 +4038,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5836,7 +5857,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5871,7 +5892,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6048,7 +6069,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6058,7 +6079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
       <selection activeCell="V209" sqref="V209"/>
     </sheetView>
   </sheetViews>

</xml_diff>